<commit_message>
fix issue with coloring for site prs, change rehab def dataframe
</commit_message>
<xml_diff>
--- a/tmp/czech_mapping.xlsx
+++ b/tmp/czech_mapping.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q1007798\Documents\Robert\Data &amp; Documents\RESQ\RES-Q support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Anaconda3\Lib\site-packages\resqdb\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C13A9C4-F3B9-4847-A6A9-76551595C194}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" xr2:uid="{50E59D78-9350-41EE-B8E6-24A347655B11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +496,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -919,22 +918,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2078E47D-88DE-46C4-9EDF-D30DD7BCAAFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="1"/>
-    <col min="4" max="4" width="35.21875" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -948,7 +947,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -960,7 +959,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -972,7 +971,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -984,7 +983,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -996,7 +995,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1079,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1091,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -1152,7 +1151,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1200,7 +1199,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1223,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1235,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
@@ -1296,7 +1295,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
@@ -1329,10 +1328,10 @@
         <v>96</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>41</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -1500,7 +1499,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -1524,7 +1523,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -1560,7 +1559,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1572,7 +1571,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -1584,7 +1583,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>55</v>
       </c>
@@ -1592,7 +1591,7 @@
       <c r="C55" s="8"/>
       <c r="D55" s="9"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>56</v>
       </c>
@@ -1600,321 +1599,321 @@
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
       <c r="D60" s="9"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
     </row>
-    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
     </row>
-    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
     </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
     </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
     </row>
-    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
     </row>
-    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
     </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
     </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
     </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
     </row>
-    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
     </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
     </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
     </row>
-    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
     </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
     </row>
-    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
     </row>
-    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
     </row>
-    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
     </row>
-    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
     </row>
-    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
     </row>
-    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
     </row>
-    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
     </row>
-    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
     </row>
-    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
     </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
     </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
     </row>
-    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
     </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
     </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
     </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
     </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
     </row>
-    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
     </row>
-    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
     </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
     </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
     </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
     </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
     </row>
-    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
     </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
     </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
     </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
     </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
     </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
     </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
   </sheetData>

</xml_diff>